<commit_message>
zapis cene kolicine v excel
</commit_message>
<xml_diff>
--- a/popis.xlsx
+++ b/popis.xlsx
@@ -373,7 +373,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +426,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>Hladilni agregat Climaveneta i-BX M 004M</t>
+          <t>Hladilni agregat Climaveneta NECS SL 1314</t>
         </is>
       </c>
       <c r="C3" s="3" t="n"/>
@@ -467,246 +467,106 @@
     <row r="9">
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>Hladilna moč:    4,300 kW</t>
+          <t>Hladilna moč:    332,3 kW</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">EER (EN14511 metoda):    2,82 </t>
+          <t xml:space="preserve">EER (EN14511 metoda):    2,55 </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">ESEER (EN14511 metoda):    4,53 </t>
+          <t xml:space="preserve">ESEER (EN14511 metoda):    4,10 </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">SEER (Reg. EU 2016/2281):    4,38 </t>
+          <t xml:space="preserve">SEER (Reg. EU 2016/2281):    4,03 </t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">El. priključek:    230V/ 1F/ 50Hz </t>
+          <t xml:space="preserve">El. priključek:    400V/ 3F/ 50Hz </t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>Zvočni tlak (SPL):    33 dB(A)</t>
+          <t>Zvočni tlak (SPL):    54 dB(A)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>Zvočna moč (PWL):    64 dB(A)</t>
+          <t>Zvočna moč (PWL):    86 dB(A)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Število hladilnih krogov:    1 </t>
+          <t xml:space="preserve">Število hladilnih krogov:    2 </t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Število kompresorjev:    1 </t>
+          <t xml:space="preserve">Število kompresorjev:    4 </t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>Dolžina:    900 mm</t>
+          <t>Dolžina:    5080 mm</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>Širina:    370 mm</t>
+          <t>Širina:    2260 mm</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>Višina:    940 mm</t>
+          <t>Višina:    2450 mm</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>Teža:    75 kg</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5" t="n"/>
-      <c r="E21" s="5" t="n"/>
-    </row>
-    <row r="22">
-      <c r="B22" s="2" t="n"/>
-    </row>
-    <row r="23">
-      <c r="B23" s="2" t="n"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="3" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="B24" s="4" t="inlineStr">
-        <is>
-          <t>Hladilni agregat Climaveneta i-BX T 035T</t>
-        </is>
-      </c>
-      <c r="C24" s="3" t="n"/>
-      <c r="D24" s="3" t="n"/>
-      <c r="E24" s="3" t="n"/>
-    </row>
-    <row r="25">
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>***Splošni opis enote***</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>PROIZVAJALEC: Mitsubishi Electric Hydronics &amp; IT Cooling Systems S.p.A, Italija</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="2" t="inlineStr">
-        <is>
-          <t>UVOZNIK: REAM d.o.o., Trzin</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" s="2" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>TEHNIČNI PODATKI:</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>Hladilna moč:    35,20 kW</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EER (EN14511 metoda):    3,01 </t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ESEER (EN14511 metoda):    4,39 </t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SEER (Reg. EU 2016/2281):    4,57 </t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">El. priključek:    400V/ 3F/ 50Hz </t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" s="2" t="inlineStr">
-        <is>
-          <t>Zvočni tlak (SPL):    45 dB(A)</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" s="2" t="inlineStr">
-        <is>
-          <t>Zvočna moč (PWL):    77 dB(A)</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Število hladilnih krogov:    1 </t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Število kompresorjev:    1 </t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" s="2" t="inlineStr">
-        <is>
-          <t>Dolžina:    1700 mm</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" s="2" t="inlineStr">
-        <is>
-          <t>Širina:    650 mm</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" s="2" t="inlineStr">
-        <is>
-          <t>Višina:    1700 mm</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" s="2" t="inlineStr">
-        <is>
-          <t>Teža:    305 kg</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>1</v>
-      </c>
-      <c r="D42" s="5" t="n"/>
-      <c r="E42" s="5" t="n"/>
+          <t>Teža:    3060 kg</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E21" s="5" t="n">
+        <v>2000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>